<commit_message>
finished parseDyd initial attempt at generic govs.
</commit_message>
<xml_diff>
--- a/tests/GovType/results01.xlsx
+++ b/tests/GovType/results01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>unknown</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>Percent of Gens with useful turbine type flag</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>steam</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>LTDtype?</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -428,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:G27"/>
+  <dimension ref="B4:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +455,10 @@
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
@@ -450,7 +468,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>2018</v>
       </c>
@@ -461,7 +479,10 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -475,7 +496,10 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -492,7 +516,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -509,7 +536,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -526,7 +556,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -543,7 +576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>5</v>
       </c>
@@ -560,7 +593,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
@@ -577,7 +613,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -594,7 +633,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
@@ -611,7 +653,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
@@ -628,7 +673,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
@@ -645,7 +693,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
@@ -662,7 +713,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>12</v>
       </c>
@@ -679,7 +730,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
       <c r="C19" t="s">
         <v>13</v>
       </c>
@@ -696,7 +750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>14</v>
       </c>
@@ -713,7 +767,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>15</v>
       </c>
@@ -730,7 +784,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
       <c r="C22" t="s">
         <v>16</v>
       </c>
@@ -747,7 +804,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
       <c r="C23" t="s">
         <v>17</v>
       </c>
@@ -764,7 +824,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
@@ -781,7 +844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>19</v>
       </c>
@@ -798,7 +861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
addition of generic steam gov agent and flatlines.p
</commit_message>
<xml_diff>
--- a/tests/GovType/results01.xlsx
+++ b/tests/GovType/results01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heyth\source\repos\thadhaines\PSLTDSim\tests\GovType\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jhaines\source\Repos\thadhaines\PSLTDSim\tests\GovType\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,7 +446,7 @@
   <dimension ref="B4:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Alteration of deadband test, addition of IEEE test, update to govtype.excel
</commit_message>
<xml_diff>
--- a/tests/GovType/results01.xlsx
+++ b/tests/GovType/results01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
   <si>
     <t>unknown</t>
   </si>
@@ -111,6 +111,75 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>'steam'</t>
+  </si>
+  <si>
+    <t>'hydro'</t>
+  </si>
+  <si>
+    <t>'general'</t>
+  </si>
+  <si>
+    <t>'wind'</t>
+  </si>
+  <si>
+    <t>'loadCTRL'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'ccbt1' :  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'gast' :   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'w2301' :  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'ieeeg3' : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'ieeeg1' : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'g2wscc' : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'hyg3' :   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'hygov4' : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'hygov' :  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'hygovr' : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'pidgov' : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'ggov1' :  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'ggov3' :  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'wndtge' : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'wndtrb' : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'lcfb1' :  </t>
+  </si>
+  <si>
+    <t>Gov Model</t>
+  </si>
+  <si>
+    <t>PSLF Manual Description</t>
   </si>
 </sst>
 </file>
@@ -134,12 +203,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -154,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -163,6 +244,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,74 +527,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G27"/>
+  <dimension ref="B2:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection sqref="A1:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2014</v>
+      </c>
+    </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>938</v>
+      </c>
+      <c r="E4">
+        <v>1759</v>
+      </c>
+      <c r="F4">
+        <v>2047</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="2">
-        <v>2018</v>
-      </c>
-      <c r="E5" s="2">
-        <v>2016</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2014</v>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>219</v>
+      </c>
+      <c r="E5">
+        <v>187</v>
+      </c>
+      <c r="F5">
+        <v>147</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>938</v>
+        <v>337</v>
       </c>
       <c r="E6">
-        <v>1759</v>
+        <v>274</v>
       </c>
       <c r="F6">
-        <v>2047</v>
+        <v>161</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>219</v>
+        <v>167</v>
       </c>
       <c r="E7">
-        <v>187</v>
+        <v>112</v>
       </c>
       <c r="F7">
-        <v>147</v>
+        <v>71</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -521,36 +646,34 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>337</v>
+        <v>53</v>
       </c>
       <c r="E8">
-        <v>274</v>
+        <v>33</v>
       </c>
       <c r="F8">
-        <v>161</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
+      <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>167</v>
+        <v>42</v>
       </c>
       <c r="E9">
-        <v>112</v>
+        <v>41</v>
       </c>
       <c r="F9">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
@@ -558,96 +681,99 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="E10">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="F10">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>46</v>
+      </c>
+      <c r="E11">
+        <v>55</v>
+      </c>
+      <c r="F11">
+        <v>55</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>13</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>141</v>
+      </c>
+      <c r="E13">
+        <v>60</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>57</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14">
         <v>23</v>
-      </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>42</v>
-      </c>
-      <c r="E11">
-        <v>41</v>
-      </c>
-      <c r="F11">
-        <v>50</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>122</v>
-      </c>
-      <c r="E12">
-        <v>93</v>
-      </c>
-      <c r="F12">
-        <v>67</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13">
-        <v>46</v>
-      </c>
-      <c r="E13">
-        <v>55</v>
-      </c>
-      <c r="F13">
-        <v>55</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>13</v>
-      </c>
-      <c r="F14">
-        <v>9</v>
       </c>
       <c r="G14" t="s">
         <v>20</v>
@@ -655,39 +781,37 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>299</v>
+      </c>
+      <c r="E16">
+        <v>116</v>
+      </c>
+      <c r="F16">
         <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15">
-        <v>141</v>
-      </c>
-      <c r="E15">
-        <v>60</v>
-      </c>
-      <c r="F15">
-        <v>50</v>
-      </c>
-      <c r="G15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>57</v>
-      </c>
-      <c r="E16">
-        <v>30</v>
-      </c>
-      <c r="F16">
-        <v>23</v>
       </c>
       <c r="G16" t="s">
         <v>20</v>
@@ -698,87 +822,92 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D17">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="E17">
-        <v>20</v>
+        <v>105</v>
       </c>
       <c r="F17">
+        <v>74</v>
+      </c>
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
         <v>4</v>
       </c>
-      <c r="G17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>299</v>
-      </c>
-      <c r="E18">
-        <v>116</v>
-      </c>
       <c r="F18">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="G18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
+      <c r="B19" s="5"/>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D19">
-        <v>134</v>
+        <v>210</v>
       </c>
       <c r="E19">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="G19" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20">
-        <v>6</v>
+        <v>1198</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>1058</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>955</v>
       </c>
       <c r="G20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D21">
-        <v>210</v>
+        <v>91</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="G21" t="s">
         <v>20</v>
@@ -786,98 +915,248 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D22">
-        <v>1198</v>
+        <v>44</v>
       </c>
       <c r="E22">
-        <v>1058</v>
+        <v>20</v>
       </c>
       <c r="F22">
-        <v>955</v>
+        <v>8</v>
       </c>
       <c r="G22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
+      <c r="B23" s="5"/>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D23">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="E23">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24">
-        <v>44</v>
-      </c>
-      <c r="E24">
-        <v>20</v>
-      </c>
-      <c r="F24">
-        <v>8</v>
-      </c>
-      <c r="G24" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D25">
-        <v>56</v>
-      </c>
-      <c r="E25">
+        <v>76.510000000000005</v>
+      </c>
+      <c r="E25" s="1">
+        <v>56.71</v>
+      </c>
+      <c r="F25">
+        <v>46.83</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="4">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31">
         <v>0</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27">
-        <v>76.510000000000005</v>
-      </c>
-      <c r="E27" s="1">
-        <v>56.71</v>
-      </c>
-      <c r="F27">
-        <v>46.83</v>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>